<commit_message>
Bug report and test cases of admin module are updated
Bug report and test cases of admin module are updated
</commit_message>
<xml_diff>
--- a/Testing/Bug_Report/TAWA_Bug Report.xlsx
+++ b/Testing/Bug_Report/TAWA_Bug Report.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="72">
   <si>
     <t>TC_ID</t>
   </si>
@@ -184,6 +184,70 @@
   </si>
   <si>
     <t>TAWA_Admin_016</t>
+  </si>
+  <si>
+    <t>TAWA_Admin_Bug_008</t>
+  </si>
+  <si>
+    <t>TAWA_Admin_Bug_009</t>
+  </si>
+  <si>
+    <t>TAWA_Admin_Bug_010</t>
+  </si>
+  <si>
+    <t>TAWA_Admin_019</t>
+  </si>
+  <si>
+    <t>Press logout</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The ‘admin shall be redirected to login page</t>
+  </si>
+  <si>
+    <t>No action happens after pressing logout</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>TAWA_Admin_020</t>
+  </si>
+  <si>
+    <t>1- Type an existing username in the search bar
+2- Press search
+3- Press Edit
+4- Update the current username to a new one
+5- Press update
+6- Press back to "all users Page"
+7- Search for the new user name</t>
+  </si>
+  <si>
+    <t>The new shall exist in the list</t>
+  </si>
+  <si>
+    <t>The new user doesn't exist in the list</t>
+  </si>
+  <si>
+    <t>TAWA_Admin_021</t>
+  </si>
+  <si>
+    <t>1- Type an existing username in the search bar
+2- Press search
+3- Press Edit
+4- Update the current username to a new one
+5-Press Update</t>
+  </si>
+  <si>
+    <t>The admin shall be redirected to "successfully added" page</t>
+  </si>
+  <si>
+    <t>No action happens after pressing update</t>
+  </si>
+  <si>
+    <t>The new user doesn't exist in the list after editing</t>
+  </si>
+  <si>
+    <t>No action happens after pressing update user</t>
   </si>
 </sst>
 </file>
@@ -540,10 +604,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -866,6 +930,120 @@
         <v>13</v>
       </c>
     </row>
+    <row r="9" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" t="s">
+        <v>60</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F9" t="s">
+        <v>59</v>
+      </c>
+      <c r="G9" t="s">
+        <v>60</v>
+      </c>
+      <c r="H9" t="s">
+        <v>61</v>
+      </c>
+      <c r="I9" t="s">
+        <v>61</v>
+      </c>
+      <c r="J9" t="s">
+        <v>21</v>
+      </c>
+      <c r="K9" t="s">
+        <v>14</v>
+      </c>
+      <c r="L9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" t="s">
+        <v>70</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F10" t="s">
+        <v>64</v>
+      </c>
+      <c r="G10" t="s">
+        <v>65</v>
+      </c>
+      <c r="H10" t="s">
+        <v>61</v>
+      </c>
+      <c r="I10" t="s">
+        <v>61</v>
+      </c>
+      <c r="J10" t="s">
+        <v>21</v>
+      </c>
+      <c r="K10" t="s">
+        <v>14</v>
+      </c>
+      <c r="L10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11" t="s">
+        <v>71</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="F11" t="s">
+        <v>68</v>
+      </c>
+      <c r="G11" t="s">
+        <v>69</v>
+      </c>
+      <c r="H11" t="s">
+        <v>26</v>
+      </c>
+      <c r="I11" t="s">
+        <v>26</v>
+      </c>
+      <c r="J11" t="s">
+        <v>21</v>
+      </c>
+      <c r="K11" t="s">
+        <v>14</v>
+      </c>
+      <c r="L11" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update test cases after execution and report bugs
</commit_message>
<xml_diff>
--- a/Testing/Bug_Report/TAWA_Bug Report.xlsx
+++ b/Testing/Bug_Report/TAWA_Bug Report.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="92">
   <si>
     <t>TC_ID</t>
   </si>
@@ -248,6 +248,71 @@
   </si>
   <si>
     <t>No action happens after pressing update user</t>
+  </si>
+  <si>
+    <t>Tawa-Logout_Bug_011</t>
+  </si>
+  <si>
+    <t>TAWA_Logout_002</t>
+  </si>
+  <si>
+    <t>Admin still in admin page after clicking on "log out" button instead of redirected to login page.</t>
+  </si>
+  <si>
+    <t>1-Click on "Logout" link in page Header in Admin page</t>
+  </si>
+  <si>
+    <t>Admin shall be logged in</t>
+  </si>
+  <si>
+    <t>Admin shall be logged out and redirected to Home Page</t>
+  </si>
+  <si>
+    <t>Admin still in Admin Page</t>
+  </si>
+  <si>
+    <t>TAWA_SignUp_003</t>
+  </si>
+  <si>
+    <t>Tawa-SignUp_Bug_012</t>
+  </si>
+  <si>
+    <t>System Accepts any length from the user in Full name field</t>
+  </si>
+  <si>
+    <t>1-Open TAWA Website.
+2-Click on signup link in page Header.
+3-Choose "User"Radio buton.
+4-Enter Full name with length &gt; 24 char.
+5-Enter all reset fields with valid data.
+6-Click on "SignUp" button.</t>
+  </si>
+  <si>
+    <t>An error message shall appear with "The data entered were invalid, Please re-enter your data".</t>
+  </si>
+  <si>
+    <t>The system accepts the entered data and redirected the user to login page.</t>
+  </si>
+  <si>
+    <t>TAWA_SignUp_004</t>
+  </si>
+  <si>
+    <t>Tawa-SignUp_Bug_013</t>
+  </si>
+  <si>
+    <t>Tawa-SignUp_Bug_014</t>
+  </si>
+  <si>
+    <t>Tawa-SignUp_Bug_015</t>
+  </si>
+  <si>
+    <t>Tawa-SignUp_Bug_016</t>
+  </si>
+  <si>
+    <t>The Successful message doesn't appear and user redirected immediately to login page.</t>
+  </si>
+  <si>
+    <t>The user shall sign up successfully and message appear with " Congratulations! A new account has been created successfully", then user shall redirected to login page.</t>
   </si>
 </sst>
 </file>
@@ -263,7 +328,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -276,8 +341,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -285,19 +356,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -604,444 +693,532 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="E11" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.85546875" customWidth="1"/>
-    <col min="2" max="2" width="20.28515625" customWidth="1"/>
-    <col min="3" max="3" width="33" customWidth="1"/>
-    <col min="4" max="4" width="29.42578125" customWidth="1"/>
-    <col min="5" max="5" width="32.5703125" customWidth="1"/>
-    <col min="6" max="6" width="34.28515625" customWidth="1"/>
-    <col min="7" max="7" width="32.5703125" customWidth="1"/>
-    <col min="8" max="8" width="17" customWidth="1"/>
-    <col min="9" max="9" width="22.85546875" customWidth="1"/>
-    <col min="10" max="10" width="25.140625" customWidth="1"/>
-    <col min="11" max="11" width="15.7109375" customWidth="1"/>
-    <col min="12" max="12" width="31.42578125" customWidth="1"/>
+    <col min="1" max="1" width="22.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="33" style="1" customWidth="1"/>
+    <col min="4" max="4" width="29.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="32.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="34.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="32.5703125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="17" style="1" customWidth="1"/>
+    <col min="9" max="9" width="22.85546875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="25.140625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" style="1" customWidth="1"/>
+    <col min="12" max="12" width="31.42578125" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L3" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L4" t="s">
+      <c r="L4" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="K5" t="s">
+      <c r="K5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L5" t="s">
+      <c r="L5" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="K6" t="s">
+      <c r="K6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L6" t="s">
+      <c r="L6" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J7" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="K7" t="s">
+      <c r="K7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L7" t="s">
+      <c r="L7" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I8" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J8" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="K8" t="s">
+      <c r="K8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L8" t="s">
+      <c r="L8" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I9" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="K9" t="s">
+      <c r="K9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L9" t="s">
+      <c r="L9" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="135" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H10" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I10" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="J10" t="s">
+      <c r="J10" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="K10" t="s">
+      <c r="K10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L10" t="s">
+      <c r="L10" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="105" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E11" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H11" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I11" t="s">
+      <c r="I11" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="J11" t="s">
+      <c r="J11" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="K11" t="s">
+      <c r="K11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L11" t="s">
+      <c r="L11" s="1" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
maysoon bugs is added
</commit_message>
<xml_diff>
--- a/Testing/Bug_Report/TAWA_Bug Report.xlsx
+++ b/Testing/Bug_Report/TAWA_Bug Report.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="AdminPage_Bugs" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="129">
   <si>
     <t>TC_ID</t>
   </si>
@@ -300,19 +300,162 @@
     <t>Tawa-SignUp_Bug_013</t>
   </si>
   <si>
-    <t>Tawa-SignUp_Bug_014</t>
-  </si>
-  <si>
-    <t>Tawa-SignUp_Bug_015</t>
-  </si>
-  <si>
-    <t>Tawa-SignUp_Bug_016</t>
-  </si>
-  <si>
     <t>The Successful message doesn't appear and user redirected immediately to login page.</t>
   </si>
   <si>
     <t>The user shall sign up successfully and message appear with " Congratulations! A new account has been created successfully", then user shall redirected to login page.</t>
+  </si>
+  <si>
+    <t>TAWA_HomePage_003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">there is no sign up button in the home page navigation bar </t>
+  </si>
+  <si>
+    <t>1-Go to (Travel-Adviser-Web-Application/UI/Log-Reg-UI/login.php)
+2- Enter valid user Credentials
+3- check the home page navigation bar</t>
+  </si>
+  <si>
+    <t>1-go to the website url
+2-the home page will open 
+3- check that the navigation bar has sign up button</t>
+  </si>
+  <si>
+    <t>the home page shall contain sign up button 
+in the navigation bar</t>
+  </si>
+  <si>
+    <t>the navigation bar is contained
+ signup link not button</t>
+  </si>
+  <si>
+    <t>Maysoon Magdy</t>
+  </si>
+  <si>
+    <t>TAWA_HomePage_006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">there is no login  button in the home page navigation bar </t>
+  </si>
+  <si>
+    <t>1-go to the website url
+2-the home page will open 
+3- check that the navigation bar has login button</t>
+  </si>
+  <si>
+    <t>the home page shall contain login button 
+in the navigation bar</t>
+  </si>
+  <si>
+    <t>the navigation bar is contained
+ login link not button</t>
+  </si>
+  <si>
+    <t>TAWA_HomePage_007</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> the home page doesn't contains a photo gallery of the top travel destinations.</t>
+  </si>
+  <si>
+    <t>1-go to the website url
+2-the home page will open 
+3- check the  a photo gallery of the top travel destinations.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the home page shall  contain a photo gallery of
+ the top travel destinations. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">the home page doesn't contain
+ the photo gallery </t>
+  </si>
+  <si>
+    <t>Hight</t>
+  </si>
+  <si>
+    <t>TAWA_Destination_002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">there is no list of the best restaurant </t>
+  </si>
+  <si>
+    <t>1-go to the website url
+2-the home page will open 
+3-click on Read more button in the destinations 
+4- the user will be redirected to the destination detailes page
+5- check the list of the best restaurants</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the user will find a list 
+of the best restaurants </t>
+  </si>
+  <si>
+    <t xml:space="preserve">there is no list of best restaurant </t>
+  </si>
+  <si>
+    <t>TAWA_Destination_003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">there is no list of the available airlines </t>
+  </si>
+  <si>
+    <t>1-go to the website url
+2-the home page will open 
+3-click on Read more button in the destinations 
+4- the user will be redirected to the destination detailes page
+5- check the list of the available airlines</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the user will find a list 
+of available places </t>
+  </si>
+  <si>
+    <t>there is no list of  available airlines</t>
+  </si>
+  <si>
+    <t>TAWA_Destination_007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the unautherized user could see the feedback , rating , and book now buttons </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-Go to (Travel-Adviser-Web-Application/UI/Log-Reg-UI/login.php)
+2- goto the home page
+3- click on anu of the destination page 
+4- check the content  </t>
+  </si>
+  <si>
+    <t>1-go to the website url
+2-the home page will open 
+3-click on Read more button in the destinations 
+4- the user will be redirected to the destination detailes page
+5- check book button
+6- check feedback button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">there is no buttons </t>
+  </si>
+  <si>
+    <t xml:space="preserve">buttons are exsisted </t>
+  </si>
+  <si>
+    <t>Tawa-HomePage_Bug_014</t>
+  </si>
+  <si>
+    <t>Tawa-HomePage_Bug_015</t>
+  </si>
+  <si>
+    <t>Tawa-HomePage_Bug_016</t>
+  </si>
+  <si>
+    <t>Tawa-Destination_Bug_017</t>
+  </si>
+  <si>
+    <t>Tawa-Destination_Bug_018</t>
+  </si>
+  <si>
+    <t>Tawa-Destination_Bug_019</t>
   </si>
 </sst>
 </file>
@@ -375,7 +518,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -388,6 +531,42 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -693,30 +872,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E11" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="20.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="20.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="33" style="1" customWidth="1"/>
-    <col min="4" max="4" width="29.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="32.5703125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="34.28515625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="32.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="29.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="32.5546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="34.33203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="32.5546875" style="1" customWidth="1"/>
     <col min="8" max="8" width="17" style="1" customWidth="1"/>
-    <col min="9" max="9" width="22.85546875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="25.140625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="15.7109375" style="1" customWidth="1"/>
-    <col min="12" max="12" width="31.42578125" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="1"/>
+    <col min="9" max="9" width="22.88671875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="25.109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="15.6640625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="31.44140625" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>33</v>
       </c>
@@ -754,7 +933,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
@@ -792,7 +971,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>28</v>
       </c>
@@ -830,7 +1009,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>32</v>
       </c>
@@ -868,7 +1047,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -906,7 +1085,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>34</v>
       </c>
@@ -944,7 +1123,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>35</v>
       </c>
@@ -982,7 +1161,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>36</v>
       </c>
@@ -1020,7 +1199,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>54</v>
       </c>
@@ -1058,7 +1237,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>55</v>
       </c>
@@ -1096,7 +1275,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>56</v>
       </c>
@@ -1134,7 +1313,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>72</v>
       </c>
@@ -1163,7 +1342,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>80</v>
       </c>
@@ -1189,7 +1368,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="72" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>86</v>
       </c>
@@ -1197,28 +1376,241 @@
         <v>85</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C15" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="D15" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="G14" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E15" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="J15" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="K15" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="L15" s="6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="H16" t="s">
+        <v>20</v>
+      </c>
+      <c r="I16" t="s">
+        <v>20</v>
+      </c>
+      <c r="J16" t="s">
+        <v>27</v>
+      </c>
+      <c r="K16" t="s">
+        <v>14</v>
+      </c>
+      <c r="L16" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>89</v>
+        <v>125</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="H17" t="s">
+        <v>106</v>
+      </c>
+      <c r="I17" t="s">
+        <v>26</v>
+      </c>
+      <c r="J17" t="s">
+        <v>21</v>
+      </c>
+      <c r="K17" t="s">
+        <v>14</v>
+      </c>
+      <c r="L17" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="F18" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="G18" t="s">
+        <v>111</v>
+      </c>
+      <c r="H18" t="s">
+        <v>26</v>
+      </c>
+      <c r="I18" t="s">
+        <v>26</v>
+      </c>
+      <c r="J18" t="s">
+        <v>21</v>
+      </c>
+      <c r="K18" t="s">
+        <v>14</v>
+      </c>
+      <c r="L18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="F19" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="G19" t="s">
+        <v>116</v>
+      </c>
+      <c r="H19" t="s">
+        <v>106</v>
+      </c>
+      <c r="I19" t="s">
+        <v>106</v>
+      </c>
+      <c r="J19" t="s">
+        <v>21</v>
+      </c>
+      <c r="K19" t="s">
+        <v>14</v>
+      </c>
+      <c r="L19" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="E20" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="F20" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="G20" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="H20" t="s">
+        <v>106</v>
+      </c>
+      <c r="I20" t="s">
+        <v>106</v>
+      </c>
+      <c r="J20" t="s">
+        <v>21</v>
+      </c>
+      <c r="K20" t="s">
+        <v>14</v>
+      </c>
+      <c r="L20" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update test cases and bug report
</commit_message>
<xml_diff>
--- a/Testing/Bug_Report/TAWA_Bug Report.xlsx
+++ b/Testing/Bug_Report/TAWA_Bug Report.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="AdminPage_Bugs" sheetId="1" r:id="rId1"/>
+    <sheet name="SignUp_Logout_Pages Bugs" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="139">
   <si>
     <t>TC_ID</t>
   </si>
@@ -250,9 +251,6 @@
     <t>No action happens after pressing update user</t>
   </si>
   <si>
-    <t>Tawa-Logout_Bug_011</t>
-  </si>
-  <si>
     <t>TAWA_Logout_002</t>
   </si>
   <si>
@@ -271,13 +269,7 @@
     <t>Admin still in Admin Page</t>
   </si>
   <si>
-    <t>TAWA_SignUp_003</t>
-  </si>
-  <si>
     <t>Tawa-SignUp_Bug_012</t>
-  </si>
-  <si>
-    <t>System Accepts any length from the user in Full name field</t>
   </si>
   <si>
     <t>1-Open TAWA Website.
@@ -294,33 +286,263 @@
     <t>The system accepts the entered data and redirected the user to login page.</t>
   </si>
   <si>
-    <t>TAWA_SignUp_004</t>
-  </si>
-  <si>
     <t>Tawa-SignUp_Bug_013</t>
   </si>
   <si>
-    <t>Tawa-SignUp_Bug_014</t>
-  </si>
-  <si>
-    <t>Tawa-SignUp_Bug_015</t>
-  </si>
-  <si>
-    <t>Tawa-SignUp_Bug_016</t>
-  </si>
-  <si>
-    <t>The Successful message doesn't appear and user redirected immediately to login page.</t>
-  </si>
-  <si>
-    <t>The user shall sign up successfully and message appear with " Congratulations! A new account has been created successfully", then user shall redirected to login page.</t>
+    <t>Full name field accepts any type of inputs instead of accepting characters and spaces only</t>
+  </si>
+  <si>
+    <t>1-Open TAWA Website.
+2-Click on signup link in page Header.
+3-Choose "User"Radio buton.
+4-Enter full name with characters ,spaces and numbers/special characters.
+5-Enter all reset fields with valid data.
+6-Click on "SignUp" button.</t>
+  </si>
+  <si>
+    <t>An error message should appear with "The data entered were invalid, Please re-enter your data"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Full name field accepts any length </t>
+  </si>
+  <si>
+    <t xml:space="preserve">User name field accepts any length </t>
+  </si>
+  <si>
+    <t>1-Open TAWA Website.
+2-Click on signup link in page Header.
+3-Choose "User"Radio buton.
+4-Enter User name woth length &gt; 14 char.
+5-Enter all reset fields with valid data.
+6-Click on "SignUp" button.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User name field accepts spaces </t>
+  </si>
+  <si>
+    <t>1-Open TAWA Website.
+2-Click on signup link in page Header.
+3-Choose "User"Radio buton.
+4-Enter User name with characters ,spaces and numbers/special characters.
+5-Enter all reset fields with valid data.
+6-Click on "SignUp" button.</t>
+  </si>
+  <si>
+    <t>Nesma Bahgat</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>User name field accepts spaces and redirects user to login page</t>
+  </si>
+  <si>
+    <t>email field accepts any length</t>
+  </si>
+  <si>
+    <t>1-Open TAWA Website.
+2-Click on signup link in page Header.
+3-Choose "User"Radio buton.
+4-Enter email with length &gt; 24 char.
+5-Enter all reset fields with valid data.
+6-Click on "SignUp" button.</t>
+  </si>
+  <si>
+    <t>email field accepts format without "." char</t>
+  </si>
+  <si>
+    <t>1-Open TAWA Website.
+2-Click on signup link in page Header.
+3-Choose "User"Radio buton.
+4-Enter email without . char.
+5-Enter all reset fields with valid data.
+6-Click on "SignUp" button.</t>
+  </si>
+  <si>
+    <t>An error message should appear restricted to email fromat with "." char.</t>
+  </si>
+  <si>
+    <t>User redirected to login page without any error messages</t>
+  </si>
+  <si>
+    <t>phone field accepts any length</t>
+  </si>
+  <si>
+    <t>1-Open TAWA Website.
+2-Click on signup link in page Header.
+3-Choose "User"Radio buton.
+4-Enter phone number &gt; 20 number.
+5-Enter all reset fields with valid data.
+6-Click on "SignUp" button.</t>
+  </si>
+  <si>
+    <t>Phone field accepts characters as an input</t>
+  </si>
+  <si>
+    <t>1-Open TAWA Website.
+2-Click on signup link in page Header.
+3-Choose "User"Radio buton.
+4-Enter phone number with numbers and characters.
+5-Enter all reset fields with valid data.
+6-Click on "SignUp" button.</t>
+  </si>
+  <si>
+    <t>Tawa-Logout_Bug_001</t>
+  </si>
+  <si>
+    <t>Tawa-SignUp_Bug_005</t>
+  </si>
+  <si>
+    <t>Tawa-SignUp_Bug_006</t>
+  </si>
+  <si>
+    <t>Tawa-SignUp_Bug_007</t>
+  </si>
+  <si>
+    <t>Tawa-SignUp_Bug_008</t>
+  </si>
+  <si>
+    <t>Tawa-SignUp_Bug_009</t>
+  </si>
+  <si>
+    <t>Tawa-SignUp_Bug_010</t>
+  </si>
+  <si>
+    <t>Phone field accepts specaial characters</t>
+  </si>
+  <si>
+    <t>1-Open TAWA Website.
+2-Click on signup link in page Header.
+3-Choose "User"Radio buton.
+4-Enter phone number with numbers and special characters.
+5-Enter all reset fields with valid data.
+6-Click on "SignUp" button.</t>
+  </si>
+  <si>
+    <t>Tawa-SignUp_Bug_011</t>
+  </si>
+  <si>
+    <t>Password field accepts input less than 8 char</t>
+  </si>
+  <si>
+    <t>1-Open TAWA Website.
+2-Click on signup link in page Header.
+3-Choose "User"Radio buton.
+4-Enterpassword less than 8 characters.
+5-Enter all reset fields with valid data.
+6-Click on "SignUp" button.</t>
+  </si>
+  <si>
+    <t>an error message preventing leaving page with "Password must contain number, special characterm upper case, lower case and more than 8 characters.</t>
+  </si>
+  <si>
+    <t>1-Open TAWA Website.
+2-Click on signup link in page Header.
+3-Choose "User"Radio buton.
+4-Enter password with characters only.
+5-Enter all reset fields with valid data.
+6-Click on "SignUp" button.</t>
+  </si>
+  <si>
+    <t>Password field accepts special characters only as an input</t>
+  </si>
+  <si>
+    <t>Passwrod field accepts characters only as an input</t>
+  </si>
+  <si>
+    <t>TAWA_SignUp_009
+Tawa-SignUp_034</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tawa-SignUp_Bug_003
+</t>
+  </si>
+  <si>
+    <t>TAWA_SignUp_007
+Tawa-SignUp_032</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tawa-SignUp_Bug_004
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tawa-SignUp_Bug_001
+</t>
+  </si>
+  <si>
+    <t>TAWA_SignUp_003
+Tawa-SignUp_028</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tawa-SignUp_Bug_002
+</t>
+  </si>
+  <si>
+    <t>TAWA_SignUp_006
+Tawa-SignUp_031</t>
+  </si>
+  <si>
+    <t>TAWA_SignUp_011
+TAWA_SignUp_036</t>
+  </si>
+  <si>
+    <t>TAWA_SignUp_013
+TAWA_SignUp_038</t>
+  </si>
+  <si>
+    <t>TAWA_SignUp_016
+TAWA_SignUp_041</t>
+  </si>
+  <si>
+    <t>TAWA_SignUp_017
+TAWA_SignUp_042</t>
+  </si>
+  <si>
+    <t>TAWA_SignUp_022
+TAWA_SignUp_047</t>
+  </si>
+  <si>
+    <t>TAWA_SignUp_021
+TAWA_SignUp_046</t>
+  </si>
+  <si>
+    <t>TAWA_SignUp_020
+TAWA_SignUp_045</t>
+  </si>
+  <si>
+    <t>TAWA_SignUp_019
+TAWA_SignUp_044</t>
+  </si>
+  <si>
+    <t>TAWA_SignUp_018
+TAWA_SignUp_043</t>
+  </si>
+  <si>
+    <t>Phone field accepts Spaces as an input</t>
+  </si>
+  <si>
+    <t>1-Open TAWA Website.
+2-Click on signup link in page Header.
+3-Choose "User"Radio buton.
+4-Enter phone number with numbers and spaces.
+5-Enter all reset fields with valid data.
+6-Click on "SignUp" button.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -375,7 +597,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -387,6 +609,9 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -693,10 +918,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E11" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E12" sqref="E12:L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1134,91 +1360,573 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.5703125" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" customWidth="1"/>
+    <col min="3" max="3" width="38.5703125" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" customWidth="1"/>
+    <col min="5" max="5" width="40.42578125" customWidth="1"/>
+    <col min="6" max="6" width="28.85546875" customWidth="1"/>
+    <col min="7" max="7" width="25.28515625" customWidth="1"/>
+    <col min="10" max="10" width="19.7109375" customWidth="1"/>
+    <col min="12" max="12" width="17.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>72</v>
+        <v>110</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>73</v>
+        <v>135</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>76</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="D12" s="1"/>
       <c r="E12" s="4" t="s">
-        <v>75</v>
+        <v>112</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="G12" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="H12" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="135" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C13" s="1" t="s">
+      <c r="B14" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="G14" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="H14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="F13" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="F14" s="4" t="s">
+      <c r="B15" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L15" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
test cases and bug report updated ( booking, reserved, header DONE)
</commit_message>
<xml_diff>
--- a/Testing/Bug_Report/TAWA_Bug Report.xlsx
+++ b/Testing/Bug_Report/TAWA_Bug Report.xlsx
@@ -4,20 +4,22 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="AdminPage_Bugs" sheetId="1" r:id="rId1"/>
     <sheet name="SignUp_Logout_Pages Bugs" sheetId="2" r:id="rId2"/>
     <sheet name="Destination bugs" sheetId="4" r:id="rId3"/>
     <sheet name="Home " sheetId="3" r:id="rId4"/>
+    <sheet name="Booking" sheetId="5" r:id="rId5"/>
+    <sheet name="Header" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="206">
   <si>
     <t>TC_ID</t>
   </si>
@@ -682,12 +684,113 @@
   <si>
     <t xml:space="preserve">buttons are exsisted </t>
   </si>
+  <si>
+    <t>TAWA_BOOKING_BUG_01</t>
+  </si>
+  <si>
+    <t>TAWA_BOOKING_05</t>
+  </si>
+  <si>
+    <t>Debit card number appears anyway without choosing debit card option</t>
+  </si>
+  <si>
+    <t>User must login with a valid account</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) Open Homepage
+2) Click on "Read More" button located beside any destination
+3) Click on "Book Flight" button
+4) Click on "Payment method" dropdown list and choose debit card
+</t>
+  </si>
+  <si>
+    <t>the ‘card number’ text field shall 
+appear</t>
+  </si>
+  <si>
+    <t>card number field exists anyway</t>
+  </si>
+  <si>
+    <t>meduim</t>
+  </si>
+  <si>
+    <t>Mahmoud Yasser</t>
+  </si>
+  <si>
+    <t>TAWA_BOOKING_BUG_02</t>
+  </si>
+  <si>
+    <t>TAWA_BOOKING_12</t>
+  </si>
+  <si>
+    <t>Debit card number accepts negative numbers</t>
+  </si>
+  <si>
+    <t>1) Open Homepage
+2) Click on "Read More" button located beside any destination
+3) Click on "Book Flight" button
+4) Enter negative in "debit card number" field
+5) complete all other fields
+6) Click on "book" button</t>
+  </si>
+  <si>
+    <t>Error message shall appear saying that it's forbidden to enter negative numbers in "debit card number" field</t>
+  </si>
+  <si>
+    <t>field accept negative</t>
+  </si>
+  <si>
+    <t>TAWA_BOOKING_BUG_03</t>
+  </si>
+  <si>
+    <t>TAWA_BOOKING_15</t>
+  </si>
+  <si>
+    <t>No error message appears when user tries to book more than one flight</t>
+  </si>
+  <si>
+    <t>1) Open Homepage
+2) Click on "Read More" button located beside any destination
+3) Click on "Book Flight" button
+4) Enter valid data and complete all fields
+5) Click on "book" button
+6) Repeat steps from 1 to 5</t>
+  </si>
+  <si>
+    <t>Error message shall appear saying
+that user has already booked one
+flight</t>
+  </si>
+  <si>
+    <t>no error message appears</t>
+  </si>
+  <si>
+    <t>TAWA_HEADER_02</t>
+  </si>
+  <si>
+    <t>Navigation bar doesn't appear in all pages but home</t>
+  </si>
+  <si>
+    <t>User must be logged in with
+a valid account</t>
+  </si>
+  <si>
+    <t>1) Open TAWA homepage
+2) Go to any destination page
+3) Click on TAWA logo</t>
+  </si>
+  <si>
+    <t>Page Shall be redirected to the home page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Navigation bar doesn't appear </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -703,8 +806,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -723,8 +833,13 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -747,11 +862,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -823,8 +950,27 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1134,24 +1280,24 @@
       <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="20.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="22.88671875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="33" style="1" customWidth="1"/>
-    <col min="4" max="4" width="29.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="32.5703125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="34.28515625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="32.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="29.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="32.5546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="34.33203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="32.5546875" style="1" customWidth="1"/>
     <col min="8" max="8" width="17" style="1" customWidth="1"/>
-    <col min="9" max="9" width="22.85546875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="25.140625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="15.7109375" style="1" customWidth="1"/>
-    <col min="12" max="12" width="31.42578125" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="1"/>
+    <col min="9" max="9" width="22.88671875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="25.109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="15.6640625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="31.44140625" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>33</v>
       </c>
@@ -1189,7 +1335,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
@@ -1227,7 +1373,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>28</v>
       </c>
@@ -1265,7 +1411,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>32</v>
       </c>
@@ -1303,7 +1449,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -1341,7 +1487,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>34</v>
       </c>
@@ -1379,7 +1525,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>35</v>
       </c>
@@ -1417,7 +1563,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>36</v>
       </c>
@@ -1455,7 +1601,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>54</v>
       </c>
@@ -1493,7 +1639,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>55</v>
       </c>
@@ -1531,7 +1677,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>56</v>
       </c>
@@ -1583,20 +1729,20 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.5703125" customWidth="1"/>
-    <col min="2" max="2" width="22.140625" customWidth="1"/>
-    <col min="3" max="3" width="38.5703125" customWidth="1"/>
-    <col min="4" max="4" width="22.140625" customWidth="1"/>
-    <col min="5" max="5" width="40.42578125" customWidth="1"/>
-    <col min="6" max="6" width="28.85546875" customWidth="1"/>
-    <col min="7" max="7" width="25.28515625" customWidth="1"/>
-    <col min="10" max="10" width="19.7109375" customWidth="1"/>
-    <col min="12" max="12" width="17.85546875" customWidth="1"/>
+    <col min="1" max="1" width="22.5546875" customWidth="1"/>
+    <col min="2" max="2" width="22.109375" customWidth="1"/>
+    <col min="3" max="3" width="38.5546875" customWidth="1"/>
+    <col min="4" max="4" width="22.109375" customWidth="1"/>
+    <col min="5" max="5" width="40.44140625" customWidth="1"/>
+    <col min="6" max="6" width="28.88671875" customWidth="1"/>
+    <col min="7" max="7" width="25.33203125" customWidth="1"/>
+    <col min="10" max="10" width="19.6640625" customWidth="1"/>
+    <col min="12" max="12" width="17.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>33</v>
       </c>
@@ -1634,7 +1780,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>104</v>
       </c>
@@ -1672,7 +1818,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>124</v>
       </c>
@@ -1708,7 +1854,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>126</v>
       </c>
@@ -1744,7 +1890,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>121</v>
       </c>
@@ -1780,7 +1926,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>123</v>
       </c>
@@ -1816,7 +1962,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>105</v>
       </c>
@@ -1852,7 +1998,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>106</v>
       </c>
@@ -1888,7 +2034,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>107</v>
       </c>
@@ -1924,7 +2070,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>108</v>
       </c>
@@ -1960,7 +2106,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>109</v>
       </c>
@@ -1996,7 +2142,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>110</v>
       </c>
@@ -2032,7 +2178,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>113</v>
       </c>
@@ -2068,7 +2214,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>78</v>
       </c>
@@ -2103,7 +2249,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>82</v>
       </c>
@@ -2147,22 +2293,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.42578125" customWidth="1"/>
-    <col min="2" max="2" width="27.5703125" customWidth="1"/>
-    <col min="3" max="3" width="54.7109375" customWidth="1"/>
-    <col min="4" max="4" width="28.28515625" customWidth="1"/>
-    <col min="5" max="5" width="32.42578125" customWidth="1"/>
-    <col min="6" max="6" width="28.42578125" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="29.44140625" customWidth="1"/>
+    <col min="2" max="2" width="27.5546875" customWidth="1"/>
+    <col min="3" max="3" width="54.6640625" customWidth="1"/>
+    <col min="4" max="4" width="28.33203125" customWidth="1"/>
+    <col min="5" max="5" width="32.44140625" customWidth="1"/>
+    <col min="6" max="6" width="28.44140625" customWidth="1"/>
+    <col min="7" max="7" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
         <v>33</v>
       </c>
@@ -2200,7 +2346,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
         <v>160</v>
       </c>
@@ -2238,7 +2384,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
         <v>166</v>
       </c>
@@ -2276,7 +2422,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
         <v>172</v>
       </c>
@@ -2327,16 +2473,16 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" style="6" customWidth="1"/>
-    <col min="2" max="2" width="30.140625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="21.5703125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="6" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="6"/>
+    <col min="1" max="1" width="22.44140625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="30.109375" style="6" customWidth="1"/>
+    <col min="3" max="3" width="21.5546875" style="6" customWidth="1"/>
+    <col min="4" max="4" width="9.109375" style="6" customWidth="1"/>
+    <col min="5" max="16384" width="9.109375" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>33</v>
       </c>
@@ -2374,7 +2520,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="300" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>139</v>
       </c>
@@ -2412,7 +2558,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="300" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>147</v>
       </c>
@@ -2450,7 +2596,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="300" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>153</v>
       </c>
@@ -2486,6 +2632,292 @@
       </c>
       <c r="L4" s="6" t="s">
         <v>146</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="60.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="39.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="25" t="s">
+        <v>179</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>180</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>181</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>182</v>
+      </c>
+      <c r="E2" s="27" t="s">
+        <v>183</v>
+      </c>
+      <c r="F2" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="G2" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="H2" s="28" t="s">
+        <v>186</v>
+      </c>
+      <c r="I2" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="J2" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="K2" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" s="28" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="25" t="s">
+        <v>188</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>189</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>190</v>
+      </c>
+      <c r="D3" s="27" t="s">
+        <v>182</v>
+      </c>
+      <c r="E3" s="27" t="s">
+        <v>191</v>
+      </c>
+      <c r="F3" s="27" t="s">
+        <v>192</v>
+      </c>
+      <c r="G3" s="26" t="s">
+        <v>193</v>
+      </c>
+      <c r="H3" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="I3" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="J3" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="K3" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="L3" s="28" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="25" t="s">
+        <v>194</v>
+      </c>
+      <c r="B4" s="26" t="s">
+        <v>195</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>196</v>
+      </c>
+      <c r="D4" s="27" t="s">
+        <v>182</v>
+      </c>
+      <c r="E4" s="27" t="s">
+        <v>197</v>
+      </c>
+      <c r="F4" s="27" t="s">
+        <v>198</v>
+      </c>
+      <c r="G4" s="26" t="s">
+        <v>199</v>
+      </c>
+      <c r="H4" s="28" t="s">
+        <v>186</v>
+      </c>
+      <c r="I4" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="J4" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="K4" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="L4" s="28" t="s">
+        <v>187</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:L2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="25" t="s">
+        <v>179</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>200</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="D2" s="30" t="s">
+        <v>202</v>
+      </c>
+      <c r="E2" s="30" t="s">
+        <v>203</v>
+      </c>
+      <c r="F2" s="30" t="s">
+        <v>204</v>
+      </c>
+      <c r="G2" s="29" t="s">
+        <v>205</v>
+      </c>
+      <c r="H2" s="28" t="s">
+        <v>186</v>
+      </c>
+      <c r="I2" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="J2" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="K2" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" s="28" t="s">
+        <v>187</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New bugs are added to the admin module
New bugs are added to the admin module
</commit_message>
<xml_diff>
--- a/Testing/Bug_Report/TAWA_Bug Report.xlsx
+++ b/Testing/Bug_Report/TAWA_Bug Report.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="AdminPage_Bugs" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="221">
   <si>
     <t>TC_ID</t>
   </si>
@@ -784,6 +784,55 @@
   </si>
   <si>
     <t xml:space="preserve">Navigation bar doesn't appear </t>
+  </si>
+  <si>
+    <t>TAWA_Admin_Bug_011</t>
+  </si>
+  <si>
+    <t>TAWA_Admin_022</t>
+  </si>
+  <si>
+    <t>1- Type an existing username in the search bar
+2- Press search
+3- Press Edit
+4- From the edit user page press back</t>
+  </si>
+  <si>
+    <t>The admin shall be redirected to Admin  page</t>
+  </si>
+  <si>
+    <t>The attached page appears</t>
+  </si>
+  <si>
+    <t>TAWA_Admin_023</t>
+  </si>
+  <si>
+    <t>TAWA_Admin_Bug_012</t>
+  </si>
+  <si>
+    <t>1- Press edit without entering a username in the search bar</t>
+  </si>
+  <si>
+    <t>The admin shall stay at the admin page</t>
+  </si>
+  <si>
+    <t>TAWA_Admin_Bug_013</t>
+  </si>
+  <si>
+    <t>TAWA_Admin_024</t>
+  </si>
+  <si>
+    <t>2- Press Add user
+4- From add user page press back</t>
+  </si>
+  <si>
+    <t>The admin isn't redirected to Admin  page after editing user</t>
+  </si>
+  <si>
+    <t>The admin isn't redirected to Admin  page after adding  user</t>
+  </si>
+  <si>
+    <t>The admin is redirected to edit page with insecured data in the fields after pressing edit</t>
   </si>
 </sst>
 </file>
@@ -984,6 +1033,143 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>336439</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>85724</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1854061</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>872741</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11833114" y="10944224"/>
+          <a:ext cx="1517622" cy="787017"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>56663</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1667377</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>752475</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11915775" y="12058163"/>
+          <a:ext cx="1248277" cy="695812"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>400049</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>100775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1704974</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>777490</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11896724" y="13054775"/>
+          <a:ext cx="1304925" cy="676715"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1273,31 +1459,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.88671875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="20.33203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="22.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" style="1" customWidth="1"/>
     <col min="3" max="3" width="33" style="1" customWidth="1"/>
-    <col min="4" max="4" width="29.44140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="32.5546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="34.33203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="32.5546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="29.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="32.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="34.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="32.5703125" style="1" customWidth="1"/>
     <col min="8" max="8" width="17" style="1" customWidth="1"/>
-    <col min="9" max="9" width="22.88671875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="25.109375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="15.6640625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="31.44140625" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.109375" style="1"/>
+    <col min="9" max="9" width="22.85546875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="25.140625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" style="1" customWidth="1"/>
+    <col min="12" max="12" width="31.42578125" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>33</v>
       </c>
@@ -1335,7 +1521,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
@@ -1373,7 +1559,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>28</v>
       </c>
@@ -1411,7 +1597,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>32</v>
       </c>
@@ -1449,7 +1635,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -1487,7 +1673,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>34</v>
       </c>
@@ -1525,7 +1711,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>35</v>
       </c>
@@ -1563,7 +1749,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>36</v>
       </c>
@@ -1601,7 +1787,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>54</v>
       </c>
@@ -1639,7 +1825,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" ht="135" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>55</v>
       </c>
@@ -1677,7 +1863,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>56</v>
       </c>
@@ -1713,11 +1899,120 @@
       </c>
       <c r="L11" s="1" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1726,23 +2021,23 @@
   <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.5546875" customWidth="1"/>
-    <col min="2" max="2" width="22.109375" customWidth="1"/>
-    <col min="3" max="3" width="38.5546875" customWidth="1"/>
-    <col min="4" max="4" width="22.109375" customWidth="1"/>
-    <col min="5" max="5" width="40.44140625" customWidth="1"/>
-    <col min="6" max="6" width="28.88671875" customWidth="1"/>
-    <col min="7" max="7" width="25.33203125" customWidth="1"/>
-    <col min="10" max="10" width="19.6640625" customWidth="1"/>
-    <col min="12" max="12" width="17.88671875" customWidth="1"/>
+    <col min="1" max="1" width="22.5703125" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" customWidth="1"/>
+    <col min="3" max="3" width="38.5703125" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" customWidth="1"/>
+    <col min="5" max="5" width="40.42578125" customWidth="1"/>
+    <col min="6" max="6" width="28.85546875" customWidth="1"/>
+    <col min="7" max="7" width="25.28515625" customWidth="1"/>
+    <col min="10" max="10" width="19.7109375" customWidth="1"/>
+    <col min="12" max="12" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>33</v>
       </c>
@@ -1780,7 +2075,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>104</v>
       </c>
@@ -1818,7 +2113,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>124</v>
       </c>
@@ -1854,7 +2149,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>126</v>
       </c>
@@ -1890,7 +2185,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>121</v>
       </c>
@@ -1926,7 +2221,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>123</v>
       </c>
@@ -1962,7 +2257,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>105</v>
       </c>
@@ -1998,7 +2293,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>106</v>
       </c>
@@ -2034,7 +2329,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>107</v>
       </c>
@@ -2070,7 +2365,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>108</v>
       </c>
@@ -2106,7 +2401,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>109</v>
       </c>
@@ -2142,7 +2437,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>110</v>
       </c>
@@ -2178,7 +2473,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>113</v>
       </c>
@@ -2214,7 +2509,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>78</v>
       </c>
@@ -2249,7 +2544,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>82</v>
       </c>
@@ -2297,18 +2592,18 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.44140625" customWidth="1"/>
-    <col min="2" max="2" width="27.5546875" customWidth="1"/>
-    <col min="3" max="3" width="54.6640625" customWidth="1"/>
-    <col min="4" max="4" width="28.33203125" customWidth="1"/>
-    <col min="5" max="5" width="32.44140625" customWidth="1"/>
-    <col min="6" max="6" width="28.44140625" customWidth="1"/>
-    <col min="7" max="7" width="9.109375" customWidth="1"/>
+    <col min="1" max="1" width="29.42578125" customWidth="1"/>
+    <col min="2" max="2" width="27.5703125" customWidth="1"/>
+    <col min="3" max="3" width="54.7109375" customWidth="1"/>
+    <col min="4" max="4" width="28.28515625" customWidth="1"/>
+    <col min="5" max="5" width="32.42578125" customWidth="1"/>
+    <col min="6" max="6" width="28.42578125" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>33</v>
       </c>
@@ -2346,7 +2641,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="120" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>160</v>
       </c>
@@ -2384,7 +2679,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="120" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>166</v>
       </c>
@@ -2422,7 +2717,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="120" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>172</v>
       </c>
@@ -2473,16 +2768,16 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.44140625" style="6" customWidth="1"/>
-    <col min="2" max="2" width="30.109375" style="6" customWidth="1"/>
-    <col min="3" max="3" width="21.5546875" style="6" customWidth="1"/>
-    <col min="4" max="4" width="9.109375" style="6" customWidth="1"/>
-    <col min="5" max="16384" width="9.109375" style="6"/>
+    <col min="1" max="1" width="22.42578125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="6" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>33</v>
       </c>
@@ -2520,7 +2815,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="259.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="300" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>139</v>
       </c>
@@ -2558,7 +2853,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="259.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="300" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>147</v>
       </c>
@@ -2596,7 +2891,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="259.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="300" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>153</v>
       </c>
@@ -2647,23 +2942,23 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="60.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="39.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="60.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="39.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>33</v>
       </c>
@@ -2701,7 +2996,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
         <v>179</v>
       </c>
@@ -2739,7 +3034,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="120" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
         <v>188</v>
       </c>
@@ -2777,7 +3072,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="A4" s="25" t="s">
         <v>194</v>
       </c>
@@ -2824,27 +3119,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="35.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>33</v>
       </c>
@@ -2882,7 +3177,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
         <v>179</v>
       </c>

</xml_diff>

<commit_message>
debit card number fixed
</commit_message>
<xml_diff>
--- a/Testing/Bug_Report/TAWA_Bug Report.xlsx
+++ b/Testing/Bug_Report/TAWA_Bug Report.xlsx
@@ -2971,7 +2971,7 @@
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3029,40 +3029,40 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="31" t="s">
         <v>179</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="32" t="s">
         <v>180</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="33" t="s">
         <v>181</v>
       </c>
-      <c r="D2" s="27" t="s">
+      <c r="D2" s="34" t="s">
         <v>182</v>
       </c>
-      <c r="E2" s="27" t="s">
+      <c r="E2" s="34" t="s">
         <v>183</v>
       </c>
-      <c r="F2" s="27" t="s">
+      <c r="F2" s="34" t="s">
         <v>184</v>
       </c>
-      <c r="G2" s="27" t="s">
+      <c r="G2" s="34" t="s">
         <v>185</v>
       </c>
-      <c r="H2" s="28" t="s">
+      <c r="H2" s="35" t="s">
         <v>186</v>
       </c>
-      <c r="I2" s="28" t="s">
+      <c r="I2" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="J2" s="28" t="s">
+      <c r="J2" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="L2" s="28" t="s">
+      <c r="K2" s="35" t="s">
+        <v>221</v>
+      </c>
+      <c r="L2" s="35" t="s">
         <v>187</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Bugs in admin module closed
a bug in admin module is closed
</commit_message>
<xml_diff>
--- a/Testing/Bug_Report/TAWA_Bug Report.xlsx
+++ b/Testing/Bug_Report/TAWA_Bug Report.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="AdminPage_Bugs" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="224">
   <si>
     <t>TC_ID</t>
   </si>
@@ -836,6 +836,12 @@
   </si>
   <si>
     <t>Fixed</t>
+  </si>
+  <si>
+    <t>high</t>
+  </si>
+  <si>
+    <t>closed</t>
   </si>
 </sst>
 </file>
@@ -873,7 +879,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -900,6 +906,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -943,7 +955,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1047,6 +1059,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1493,29 +1508,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.88671875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="20.33203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="22.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" style="1" customWidth="1"/>
     <col min="3" max="3" width="33" style="1" customWidth="1"/>
-    <col min="4" max="4" width="29.44140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="32.5546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="34.33203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="32.5546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="29.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="32.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="34.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="32.5703125" style="1" customWidth="1"/>
     <col min="8" max="8" width="17" style="1" customWidth="1"/>
-    <col min="9" max="9" width="22.88671875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="25.109375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="15.6640625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="31.44140625" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.109375" style="1"/>
+    <col min="9" max="9" width="22.85546875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="25.140625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" style="1" customWidth="1"/>
+    <col min="12" max="12" width="31.42578125" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>33</v>
       </c>
@@ -1553,7 +1568,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
@@ -1591,7 +1606,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>28</v>
       </c>
@@ -1629,7 +1644,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>32</v>
       </c>
@@ -1667,7 +1682,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -1705,7 +1720,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>34</v>
       </c>
@@ -1743,7 +1758,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>35</v>
       </c>
@@ -1781,7 +1796,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>36</v>
       </c>
@@ -1819,7 +1834,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>54</v>
       </c>
@@ -1857,7 +1872,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" ht="135" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>55</v>
       </c>
@@ -1895,7 +1910,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>56</v>
       </c>
@@ -1933,7 +1948,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="72" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>206</v>
       </c>
@@ -1971,45 +1986,45 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
+    <row r="13" spans="1:12" s="36" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A13" s="36" t="s">
         <v>212</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="36" t="s">
         <v>211</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="36" t="s">
         <v>220</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" s="36" t="s">
         <v>213</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="F13" s="36" t="s">
         <v>214</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="G13" s="36" t="s">
         <v>210</v>
       </c>
-      <c r="H13" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="J13" s="1" t="s">
+      <c r="H13" s="36" t="s">
+        <v>222</v>
+      </c>
+      <c r="I13" s="36" t="s">
+        <v>222</v>
+      </c>
+      <c r="J13" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="K13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L13" s="1" t="s">
+      <c r="K13" s="36" t="s">
+        <v>223</v>
+      </c>
+      <c r="L13" s="36" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>215</v>
       </c>
@@ -2039,6 +2054,12 @@
       </c>
       <c r="J14" s="1" t="s">
         <v>21</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -2056,20 +2077,20 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.5546875" customWidth="1"/>
-    <col min="2" max="2" width="22.109375" customWidth="1"/>
-    <col min="3" max="3" width="38.5546875" customWidth="1"/>
-    <col min="4" max="4" width="22.109375" customWidth="1"/>
-    <col min="5" max="5" width="40.44140625" customWidth="1"/>
-    <col min="6" max="6" width="28.88671875" customWidth="1"/>
-    <col min="7" max="7" width="25.33203125" customWidth="1"/>
-    <col min="10" max="10" width="19.6640625" customWidth="1"/>
-    <col min="12" max="12" width="17.88671875" customWidth="1"/>
+    <col min="1" max="1" width="22.5703125" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" customWidth="1"/>
+    <col min="3" max="3" width="38.5703125" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" customWidth="1"/>
+    <col min="5" max="5" width="40.42578125" customWidth="1"/>
+    <col min="6" max="6" width="28.85546875" customWidth="1"/>
+    <col min="7" max="7" width="25.28515625" customWidth="1"/>
+    <col min="10" max="10" width="19.7109375" customWidth="1"/>
+    <col min="12" max="12" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>33</v>
       </c>
@@ -2107,7 +2128,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>104</v>
       </c>
@@ -2145,7 +2166,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>124</v>
       </c>
@@ -2181,7 +2202,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>126</v>
       </c>
@@ -2217,7 +2238,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>121</v>
       </c>
@@ -2253,7 +2274,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>123</v>
       </c>
@@ -2289,7 +2310,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>105</v>
       </c>
@@ -2325,7 +2346,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>106</v>
       </c>
@@ -2361,7 +2382,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>107</v>
       </c>
@@ -2397,7 +2418,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>108</v>
       </c>
@@ -2433,7 +2454,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>109</v>
       </c>
@@ -2469,7 +2490,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>110</v>
       </c>
@@ -2505,7 +2526,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>113</v>
       </c>
@@ -2541,7 +2562,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>78</v>
       </c>
@@ -2576,7 +2597,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>82</v>
       </c>
@@ -2624,18 +2645,18 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.44140625" customWidth="1"/>
-    <col min="2" max="2" width="27.5546875" customWidth="1"/>
-    <col min="3" max="3" width="54.6640625" customWidth="1"/>
-    <col min="4" max="4" width="28.33203125" customWidth="1"/>
-    <col min="5" max="5" width="32.44140625" customWidth="1"/>
-    <col min="6" max="6" width="28.44140625" customWidth="1"/>
-    <col min="7" max="7" width="9.109375" customWidth="1"/>
+    <col min="1" max="1" width="29.42578125" customWidth="1"/>
+    <col min="2" max="2" width="27.5703125" customWidth="1"/>
+    <col min="3" max="3" width="54.7109375" customWidth="1"/>
+    <col min="4" max="4" width="28.28515625" customWidth="1"/>
+    <col min="5" max="5" width="32.42578125" customWidth="1"/>
+    <col min="6" max="6" width="28.42578125" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>33</v>
       </c>
@@ -2673,7 +2694,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="120" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>160</v>
       </c>
@@ -2711,7 +2732,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="120" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>166</v>
       </c>
@@ -2749,7 +2770,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="120" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>172</v>
       </c>
@@ -2800,16 +2821,16 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.44140625" style="6" customWidth="1"/>
-    <col min="2" max="2" width="30.109375" style="6" customWidth="1"/>
-    <col min="3" max="3" width="21.5546875" style="6" customWidth="1"/>
-    <col min="4" max="4" width="9.109375" style="6" customWidth="1"/>
-    <col min="5" max="16384" width="9.109375" style="6"/>
+    <col min="1" max="1" width="22.42578125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="6" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>33</v>
       </c>
@@ -2847,7 +2868,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="259.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="300" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>139</v>
       </c>
@@ -2885,7 +2906,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="259.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="300" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>147</v>
       </c>
@@ -2923,7 +2944,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="259.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="300" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>153</v>
       </c>
@@ -2970,27 +2991,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="60.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="39.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="60.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="39.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>33</v>
       </c>
@@ -3028,7 +3049,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
         <v>179</v>
       </c>
@@ -3066,7 +3087,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="120" x14ac:dyDescent="0.25">
       <c r="A3" s="31" t="s">
         <v>188</v>
       </c>
@@ -3104,7 +3125,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="A4" s="25" t="s">
         <v>194</v>
       </c>
@@ -3155,23 +3176,23 @@
       <selection sqref="A1:L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="35.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>33</v>
       </c>
@@ -3209,7 +3230,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
         <v>179</v>
       </c>

</xml_diff>